<commit_message>
allow non-integer exposed.to.hospital and exposed.to.discharge if all(use.hosp.rate)
</commit_message>
<xml_diff>
--- a/inst/extdata/template.xlsx
+++ b/inst/extdata/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Dropbox (UC Berkeley Biostat)/jsLEMMA/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFACF45E-420D-9A46-8763-C52688E7FC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ADC248-89D0-9549-8842-EB1F823634E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5840" yWindow="1820" windowWidth="26020" windowHeight="16980" activeTab="2" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
+    <workbookView xWindow="5840" yWindow="1820" windowWidth="26020" windowHeight="16980" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -667,15 +667,17 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -691,13 +693,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF7E970-76F8-6942-B4A0-7B2C1D2884B8}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1607,7 +1607,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C13:G14" xr:uid="{4DE0DCAE-C019-834F-B9C1-56C11EC5B821}">
       <formula1>$A$31:$A$32</formula1>
     </dataValidation>
@@ -1615,7 +1615,7 @@
       <formula1>43831</formula1>
       <formula2>44196</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:G7 C9:G9 C17:G17 C20:G20 C23:G23" xr:uid="{FAEE2E21-9B92-AA4A-8A06-54EDAF563E2B}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23:G23 C9:G9 C17:G17 C20:G20 C5:G5 C7:G7" xr:uid="{FAEE2E21-9B92-AA4A-8A06-54EDAF563E2B}">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
@@ -1626,6 +1626,10 @@
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:G3 C8:G8 C10:G10 C11:G14" xr:uid="{9F0C0177-DE3E-1444-856B-A1A4910CD57E}">
       <formula1>0</formula1>
       <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:G6" xr:uid="{24255A77-FFA2-BC46-B7A4-61EA8B17C188}">
+      <formula1>0</formula1>
+      <formula2>30</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1710,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9816A416-5B6A-4545-98DF-6AED7BBC6987}">
   <dimension ref="A1:R310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
@@ -1813,10 +1817,10 @@
         <v>95</v>
       </c>
       <c r="P2" s="40"/>
-      <c r="Q2" s="44" t="s">
+      <c r="Q2" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="R2" s="44"/>
+      <c r="R2" s="37"/>
     </row>
     <row r="3" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
@@ -1830,30 +1834,30 @@
         <v>100</v>
       </c>
       <c r="F3" s="42"/>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39" t="s">
+      <c r="H3" s="44"/>
+      <c r="I3" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39" t="s">
+      <c r="J3" s="45"/>
+      <c r="K3" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="39"/>
-      <c r="M3" s="38" t="s">
+      <c r="L3" s="45"/>
+      <c r="M3" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38" t="s">
+      <c r="N3" s="44"/>
+      <c r="O3" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="45" t="s">
+      <c r="P3" s="44"/>
+      <c r="Q3" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="R3" s="45"/>
+      <c r="R3" s="38"/>
     </row>
     <row r="4" spans="1:18" s="17" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
@@ -1862,10 +1866,10 @@
       <c r="B4" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="39">
         <v>0.85</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="41">
         <v>0.8</v>
       </c>
@@ -1890,10 +1894,10 @@
         <v>0.9</v>
       </c>
       <c r="P4" s="41"/>
-      <c r="Q4" s="37">
+      <c r="Q4" s="39">
         <v>0.9</v>
       </c>
-      <c r="R4" s="37"/>
+      <c r="R4" s="39"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
@@ -1902,38 +1906,38 @@
       <c r="B5" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="39">
         <v>0.4</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37">
+      <c r="D5" s="39"/>
+      <c r="E5" s="39">
         <v>0.4</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37">
+      <c r="F5" s="39"/>
+      <c r="G5" s="39">
         <v>0</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37">
+      <c r="H5" s="39"/>
+      <c r="I5" s="39">
         <v>0</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37">
+      <c r="J5" s="39"/>
+      <c r="K5" s="39">
         <v>0</v>
       </c>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37">
+      <c r="L5" s="39"/>
+      <c r="M5" s="39">
         <v>0</v>
       </c>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37">
+      <c r="N5" s="39"/>
+      <c r="O5" s="39">
         <v>0</v>
       </c>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37">
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39">
         <v>0.4</v>
       </c>
-      <c r="R5" s="37"/>
+      <c r="R5" s="39"/>
     </row>
     <row r="6" spans="1:18" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
@@ -8517,16 +8521,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="C3:D3"/>
@@ -8537,18 +8543,16 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B520" xr:uid="{140C1EC3-30A5-2448-BEAA-24AD135906D1}">

</xml_diff>